<commit_message>
Ajout page Décade et modification retour sur page Principale
</commit_message>
<xml_diff>
--- a/fichierInter2.xlsx
+++ b/fichierInter2.xlsx
@@ -7,12 +7,12 @@
     <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="2021-Normal Semaine" sheetId="1" r:id="rId4"/>
-    <sheet name="2021-Normal Décade" sheetId="2" r:id="rId5"/>
-    <sheet name="2021-Défavorable Semaine" sheetId="3" r:id="rId6"/>
-    <sheet name="2021-Défavorable Décade" sheetId="4" r:id="rId7"/>
-    <sheet name="2021-Favorable Semaine" sheetId="5" r:id="rId8"/>
-    <sheet name="2021-Favorable Décade" sheetId="6" r:id="rId9"/>
+    <sheet name="2020-Normal Semaine" sheetId="1" r:id="rId4"/>
+    <sheet name="2020-Normal Décade" sheetId="2" r:id="rId5"/>
+    <sheet name="2020-Défavorable Semaine" sheetId="3" r:id="rId6"/>
+    <sheet name="2020-Défavorable Décade" sheetId="4" r:id="rId7"/>
+    <sheet name="2020-Favorable Semaine" sheetId="5" r:id="rId8"/>
+    <sheet name="2020-Favorable Décade" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -37,163 +37,163 @@
     <t>Date début semaine</t>
   </si>
   <si>
-    <t>Potentiel de pousse_2021-Normal</t>
-  </si>
-  <si>
-    <t>07/01/2021</t>
-  </si>
-  <si>
-    <t>14/01/2021</t>
-  </si>
-  <si>
-    <t>21/01/2021</t>
-  </si>
-  <si>
-    <t>28/01/2021</t>
-  </si>
-  <si>
-    <t>04/02/2021</t>
-  </si>
-  <si>
-    <t>11/02/2021</t>
-  </si>
-  <si>
-    <t>18/02/2021</t>
-  </si>
-  <si>
-    <t>25/02/2021</t>
-  </si>
-  <si>
-    <t>04/03/2021</t>
-  </si>
-  <si>
-    <t>11/03/2021</t>
-  </si>
-  <si>
-    <t>18/03/2021</t>
-  </si>
-  <si>
-    <t>25/03/2021</t>
-  </si>
-  <si>
-    <t>01/04/2021</t>
-  </si>
-  <si>
-    <t>08/04/2021</t>
-  </si>
-  <si>
-    <t>15/04/2021</t>
-  </si>
-  <si>
-    <t>22/04/2021</t>
-  </si>
-  <si>
-    <t>29/04/2021</t>
-  </si>
-  <si>
-    <t>06/05/2021</t>
-  </si>
-  <si>
-    <t>13/05/2021</t>
-  </si>
-  <si>
-    <t>20/05/2021</t>
-  </si>
-  <si>
-    <t>27/05/2021</t>
-  </si>
-  <si>
-    <t>03/06/2021</t>
-  </si>
-  <si>
-    <t>10/06/2021</t>
-  </si>
-  <si>
-    <t>17/06/2021</t>
-  </si>
-  <si>
-    <t>24/06/2021</t>
-  </si>
-  <si>
-    <t>01/07/2021</t>
-  </si>
-  <si>
-    <t>08/07/2021</t>
-  </si>
-  <si>
-    <t>15/07/2021</t>
-  </si>
-  <si>
-    <t>22/07/2021</t>
-  </si>
-  <si>
-    <t>29/07/2021</t>
-  </si>
-  <si>
-    <t>05/08/2021</t>
-  </si>
-  <si>
-    <t>12/08/2021</t>
-  </si>
-  <si>
-    <t>19/08/2021</t>
-  </si>
-  <si>
-    <t>26/08/2021</t>
-  </si>
-  <si>
-    <t>02/09/2021</t>
-  </si>
-  <si>
-    <t>09/09/2021</t>
-  </si>
-  <si>
-    <t>16/09/2021</t>
-  </si>
-  <si>
-    <t>23/09/2021</t>
-  </si>
-  <si>
-    <t>30/09/2021</t>
-  </si>
-  <si>
-    <t>07/10/2021</t>
-  </si>
-  <si>
-    <t>14/10/2021</t>
-  </si>
-  <si>
-    <t>21/10/2021</t>
-  </si>
-  <si>
-    <t>28/10/2021</t>
-  </si>
-  <si>
-    <t>04/11/2021</t>
-  </si>
-  <si>
-    <t>11/11/2021</t>
-  </si>
-  <si>
-    <t>18/11/2021</t>
-  </si>
-  <si>
-    <t>25/11/2021</t>
-  </si>
-  <si>
-    <t>02/12/2021</t>
-  </si>
-  <si>
-    <t>09/12/2021</t>
-  </si>
-  <si>
-    <t>16/12/2021</t>
-  </si>
-  <si>
-    <t>23/12/2021</t>
-  </si>
-  <si>
-    <t>30/12/2021</t>
+    <t>Potentiel de pousse_2020-Normal</t>
+  </si>
+  <si>
+    <t>07/01/2020</t>
+  </si>
+  <si>
+    <t>14/01/2020</t>
+  </si>
+  <si>
+    <t>21/01/2020</t>
+  </si>
+  <si>
+    <t>28/01/2020</t>
+  </si>
+  <si>
+    <t>04/02/2020</t>
+  </si>
+  <si>
+    <t>11/02/2020</t>
+  </si>
+  <si>
+    <t>18/02/2020</t>
+  </si>
+  <si>
+    <t>25/02/2020</t>
+  </si>
+  <si>
+    <t>03/03/2020</t>
+  </si>
+  <si>
+    <t>10/03/2020</t>
+  </si>
+  <si>
+    <t>17/03/2020</t>
+  </si>
+  <si>
+    <t>24/03/2020</t>
+  </si>
+  <si>
+    <t>31/03/2020</t>
+  </si>
+  <si>
+    <t>07/04/2020</t>
+  </si>
+  <si>
+    <t>14/04/2020</t>
+  </si>
+  <si>
+    <t>21/04/2020</t>
+  </si>
+  <si>
+    <t>28/04/2020</t>
+  </si>
+  <si>
+    <t>05/05/2020</t>
+  </si>
+  <si>
+    <t>12/05/2020</t>
+  </si>
+  <si>
+    <t>19/05/2020</t>
+  </si>
+  <si>
+    <t>26/05/2020</t>
+  </si>
+  <si>
+    <t>02/06/2020</t>
+  </si>
+  <si>
+    <t>09/06/2020</t>
+  </si>
+  <si>
+    <t>16/06/2020</t>
+  </si>
+  <si>
+    <t>23/06/2020</t>
+  </si>
+  <si>
+    <t>30/06/2020</t>
+  </si>
+  <si>
+    <t>07/07/2020</t>
+  </si>
+  <si>
+    <t>14/07/2020</t>
+  </si>
+  <si>
+    <t>21/07/2020</t>
+  </si>
+  <si>
+    <t>28/07/2020</t>
+  </si>
+  <si>
+    <t>04/08/2020</t>
+  </si>
+  <si>
+    <t>11/08/2020</t>
+  </si>
+  <si>
+    <t>18/08/2020</t>
+  </si>
+  <si>
+    <t>25/08/2020</t>
+  </si>
+  <si>
+    <t>01/09/2020</t>
+  </si>
+  <si>
+    <t>08/09/2020</t>
+  </si>
+  <si>
+    <t>15/09/2020</t>
+  </si>
+  <si>
+    <t>22/09/2020</t>
+  </si>
+  <si>
+    <t>29/09/2020</t>
+  </si>
+  <si>
+    <t>06/10/2020</t>
+  </si>
+  <si>
+    <t>13/10/2020</t>
+  </si>
+  <si>
+    <t>20/10/2020</t>
+  </si>
+  <si>
+    <t>27/10/2020</t>
+  </si>
+  <si>
+    <t>03/11/2020</t>
+  </si>
+  <si>
+    <t>10/11/2020</t>
+  </si>
+  <si>
+    <t>17/11/2020</t>
+  </si>
+  <si>
+    <t>24/11/2020</t>
+  </si>
+  <si>
+    <t>01/12/2020</t>
+  </si>
+  <si>
+    <t>08/12/2020</t>
+  </si>
+  <si>
+    <t>15/12/2020</t>
+  </si>
+  <si>
+    <t>22/12/2020</t>
+  </si>
+  <si>
+    <t>29/12/2020</t>
   </si>
   <si>
     <t>Numéro de la décade</t>
@@ -202,103 +202,103 @@
     <t>Date début décade</t>
   </si>
   <si>
-    <t>10/01/2021</t>
-  </si>
-  <si>
-    <t>20/01/2021</t>
-  </si>
-  <si>
-    <t>30/01/2021</t>
-  </si>
-  <si>
-    <t>09/02/2021</t>
-  </si>
-  <si>
-    <t>19/02/2021</t>
-  </si>
-  <si>
-    <t>01/03/2021</t>
-  </si>
-  <si>
-    <t>21/03/2021</t>
-  </si>
-  <si>
-    <t>31/03/2021</t>
-  </si>
-  <si>
-    <t>10/04/2021</t>
-  </si>
-  <si>
-    <t>20/04/2021</t>
-  </si>
-  <si>
-    <t>30/04/2021</t>
-  </si>
-  <si>
-    <t>10/05/2021</t>
-  </si>
-  <si>
-    <t>30/05/2021</t>
-  </si>
-  <si>
-    <t>09/06/2021</t>
-  </si>
-  <si>
-    <t>19/06/2021</t>
-  </si>
-  <si>
-    <t>29/06/2021</t>
-  </si>
-  <si>
-    <t>09/07/2021</t>
-  </si>
-  <si>
-    <t>19/07/2021</t>
-  </si>
-  <si>
-    <t>08/08/2021</t>
-  </si>
-  <si>
-    <t>18/08/2021</t>
-  </si>
-  <si>
-    <t>28/08/2021</t>
-  </si>
-  <si>
-    <t>07/09/2021</t>
-  </si>
-  <si>
-    <t>17/09/2021</t>
-  </si>
-  <si>
-    <t>27/09/2021</t>
-  </si>
-  <si>
-    <t>17/10/2021</t>
-  </si>
-  <si>
-    <t>27/10/2021</t>
-  </si>
-  <si>
-    <t>06/11/2021</t>
-  </si>
-  <si>
-    <t>16/11/2021</t>
-  </si>
-  <si>
-    <t>26/11/2021</t>
-  </si>
-  <si>
-    <t>06/12/2021</t>
-  </si>
-  <si>
-    <t>26/12/2021</t>
-  </si>
-  <si>
-    <t>Potentiel de pousse_2021-Défavorable</t>
-  </si>
-  <si>
-    <t>Potentiel de pousse_2021-Favorable</t>
+    <t>10/01/2020</t>
+  </si>
+  <si>
+    <t>20/01/2020</t>
+  </si>
+  <si>
+    <t>30/01/2020</t>
+  </si>
+  <si>
+    <t>09/02/2020</t>
+  </si>
+  <si>
+    <t>19/02/2020</t>
+  </si>
+  <si>
+    <t>29/02/2020</t>
+  </si>
+  <si>
+    <t>20/03/2020</t>
+  </si>
+  <si>
+    <t>30/03/2020</t>
+  </si>
+  <si>
+    <t>09/04/2020</t>
+  </si>
+  <si>
+    <t>19/04/2020</t>
+  </si>
+  <si>
+    <t>29/04/2020</t>
+  </si>
+  <si>
+    <t>09/05/2020</t>
+  </si>
+  <si>
+    <t>29/05/2020</t>
+  </si>
+  <si>
+    <t>08/06/2020</t>
+  </si>
+  <si>
+    <t>18/06/2020</t>
+  </si>
+  <si>
+    <t>28/06/2020</t>
+  </si>
+  <si>
+    <t>08/07/2020</t>
+  </si>
+  <si>
+    <t>18/07/2020</t>
+  </si>
+  <si>
+    <t>07/08/2020</t>
+  </si>
+  <si>
+    <t>17/08/2020</t>
+  </si>
+  <si>
+    <t>27/08/2020</t>
+  </si>
+  <si>
+    <t>06/09/2020</t>
+  </si>
+  <si>
+    <t>16/09/2020</t>
+  </si>
+  <si>
+    <t>26/09/2020</t>
+  </si>
+  <si>
+    <t>16/10/2020</t>
+  </si>
+  <si>
+    <t>26/10/2020</t>
+  </si>
+  <si>
+    <t>05/11/2020</t>
+  </si>
+  <si>
+    <t>15/11/2020</t>
+  </si>
+  <si>
+    <t>25/11/2020</t>
+  </si>
+  <si>
+    <t>05/12/2020</t>
+  </si>
+  <si>
+    <t>25/12/2020</t>
+  </si>
+  <si>
+    <t>Potentiel de pousse_2020-Défavorable</t>
+  </si>
+  <si>
+    <t>Potentiel de pousse_2020-Favorable</t>
   </si>
 </sst>
 </file>
@@ -798,8 +798,12 @@
       <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="D11"/>
-      <c r="E11"/>
+      <c r="D11">
+        <v>11</v>
+      </c>
+      <c r="E11">
+        <v>3.98</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
@@ -812,10 +816,10 @@
         <v>16</v>
       </c>
       <c r="D12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E12">
-        <v>20.14</v>
+        <v>28.33</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -828,8 +832,12 @@
       <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="D13"/>
-      <c r="E13"/>
+      <c r="D13">
+        <v>7</v>
+      </c>
+      <c r="E13">
+        <v>44.39</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
@@ -842,10 +850,10 @@
         <v>18</v>
       </c>
       <c r="D14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E14">
-        <v>42.41</v>
+        <v>42.35</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -859,10 +867,10 @@
         <v>19</v>
       </c>
       <c r="D15">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E15">
-        <v>45.09</v>
+        <v>30.56</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -876,10 +884,10 @@
         <v>20</v>
       </c>
       <c r="D16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16">
-        <v>10.12</v>
+        <v>62.5</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -893,10 +901,10 @@
         <v>21</v>
       </c>
       <c r="D17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E17">
-        <v>24.43</v>
+        <v>44.05</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -910,10 +918,10 @@
         <v>22</v>
       </c>
       <c r="D18">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E18">
-        <v>8.33</v>
+        <v>30.79</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -927,10 +935,10 @@
         <v>23</v>
       </c>
       <c r="D19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19">
-        <v>57.14</v>
+        <v>43.45</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -947,7 +955,7 @@
         <v>6</v>
       </c>
       <c r="E20">
-        <v>47.02</v>
+        <v>69.45</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -961,10 +969,10 @@
         <v>25</v>
       </c>
       <c r="D21">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E21">
-        <v>30.95</v>
+        <v>47.22</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -978,10 +986,10 @@
         <v>26</v>
       </c>
       <c r="D22">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E22">
-        <v>77.78</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -995,10 +1003,10 @@
         <v>27</v>
       </c>
       <c r="D23">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E23">
-        <v>77.35</v>
+        <v>35.42</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -1012,10 +1020,10 @@
         <v>28</v>
       </c>
       <c r="D24">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E24">
-        <v>40.0</v>
+        <v>11.72</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1029,10 +1037,10 @@
         <v>29</v>
       </c>
       <c r="D25">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E25">
-        <v>10.71</v>
+        <v>11.91</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1046,10 +1054,10 @@
         <v>30</v>
       </c>
       <c r="D26">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E26">
-        <v>39.29</v>
+        <v>26.04</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1063,10 +1071,10 @@
         <v>31</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E27">
-        <v>51.19</v>
+        <v>58.73</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1080,10 +1088,10 @@
         <v>32</v>
       </c>
       <c r="D28">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E28">
-        <v>17.86</v>
+        <v>50.52</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1097,10 +1105,10 @@
         <v>33</v>
       </c>
       <c r="D29">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E29">
-        <v>26.02</v>
+        <v>17.71</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1114,10 +1122,10 @@
         <v>34</v>
       </c>
       <c r="D30">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>26.04</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1561,8 +1569,12 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8"/>
-      <c r="E8"/>
+      <c r="D8">
+        <v>11</v>
+      </c>
+      <c r="E8">
+        <v>3.98</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
@@ -1575,10 +1587,10 @@
         <v>66</v>
       </c>
       <c r="D9">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E9">
-        <v>20.14</v>
+        <v>36.36</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1592,10 +1604,10 @@
         <v>67</v>
       </c>
       <c r="D10">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E10">
-        <v>42.41</v>
+        <v>42.35</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1609,10 +1621,10 @@
         <v>68</v>
       </c>
       <c r="D11">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E11">
-        <v>27.61</v>
+        <v>46.53</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1626,10 +1638,10 @@
         <v>69</v>
       </c>
       <c r="D12">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E12">
-        <v>24.43</v>
+        <v>44.05</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1643,10 +1655,10 @@
         <v>70</v>
       </c>
       <c r="D13">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E13">
-        <v>8.33</v>
+        <v>30.79</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1660,10 +1672,10 @@
         <v>71</v>
       </c>
       <c r="D14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14">
-        <v>52.08</v>
+        <v>56.45</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1677,10 +1689,10 @@
         <v>25</v>
       </c>
       <c r="D15">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E15">
-        <v>30.95</v>
+        <v>47.22</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1694,10 +1706,10 @@
         <v>72</v>
       </c>
       <c r="D16">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E16">
-        <v>77.78</v>
+        <v>17.71</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1711,10 +1723,10 @@
         <v>73</v>
       </c>
       <c r="D17">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E17">
-        <v>58.68</v>
+        <v>11.72</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1731,7 +1743,7 @@
         <v>10</v>
       </c>
       <c r="E18">
-        <v>25.0</v>
+        <v>18.98</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1745,10 +1757,10 @@
         <v>75</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E19">
-        <v>51.19</v>
+        <v>58.73</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1762,10 +1774,10 @@
         <v>76</v>
       </c>
       <c r="D20">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E20">
-        <v>21.94</v>
+        <v>50.52</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1779,10 +1791,10 @@
         <v>77</v>
       </c>
       <c r="D21">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E21">
-        <v>26.04</v>
+        <v>8.86</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2174,8 +2186,12 @@
       <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="D11"/>
-      <c r="E11"/>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>3.13</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
@@ -2191,7 +2207,7 @@
         <v>4</v>
       </c>
       <c r="E12">
-        <v>12.5</v>
+        <v>23.96</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -2204,8 +2220,12 @@
       <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="D13"/>
-      <c r="E13"/>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>44.64</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
@@ -2218,10 +2238,10 @@
         <v>18</v>
       </c>
       <c r="D14">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E14">
-        <v>50.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2234,12 +2254,8 @@
       <c r="C15" t="s">
         <v>19</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>34.38</v>
-      </c>
+      <c r="D15"/>
+      <c r="E15"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
@@ -2251,8 +2267,12 @@
       <c r="C16" t="s">
         <v>20</v>
       </c>
-      <c r="D16"/>
-      <c r="E16"/>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>37.5</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
@@ -2265,10 +2285,10 @@
         <v>21</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E17">
-        <v>19.32</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -2285,7 +2305,7 @@
         <v>3</v>
       </c>
       <c r="E18">
-        <v>9.72</v>
+        <v>21.43</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -2299,10 +2319,10 @@
         <v>23</v>
       </c>
       <c r="D19">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E19">
-        <v>47.32</v>
+        <v>39.28</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2315,8 +2335,12 @@
       <c r="C20" t="s">
         <v>24</v>
       </c>
-      <c r="D20"/>
-      <c r="E20"/>
+      <c r="D20">
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <v>29.17</v>
+      </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" t="s">
@@ -2332,7 +2356,7 @@
         <v>2</v>
       </c>
       <c r="E21">
-        <v>57.15</v>
+        <v>29.17</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -2349,7 +2373,7 @@
         <v>2</v>
       </c>
       <c r="E22">
-        <v>77.08</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -2363,10 +2387,10 @@
         <v>27</v>
       </c>
       <c r="D23">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E23">
-        <v>20.32</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -2379,12 +2403,8 @@
       <c r="C24" t="s">
         <v>28</v>
       </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>35.0</v>
-      </c>
+      <c r="D24"/>
+      <c r="E24"/>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" t="s">
@@ -2400,7 +2420,7 @@
         <v>2</v>
       </c>
       <c r="E25">
-        <v>0.0</v>
+        <v>7.14</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -2414,10 +2434,10 @@
         <v>30</v>
       </c>
       <c r="D26">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E26">
-        <v>35.42</v>
+        <v>22.92</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -2431,10 +2451,10 @@
         <v>31</v>
       </c>
       <c r="D27">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>14.29</v>
+        <v>63.89</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -2448,10 +2468,10 @@
         <v>32</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E28">
-        <v>0.0</v>
+        <v>85.42</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -2465,10 +2485,10 @@
         <v>33</v>
       </c>
       <c r="D29">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>55.36</v>
+        <v>22.92</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -2482,10 +2502,10 @@
         <v>34</v>
       </c>
       <c r="D30">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E30">
-        <v>42.71</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -2929,8 +2949,12 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8"/>
-      <c r="E8"/>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>3.13</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
@@ -2943,10 +2967,10 @@
         <v>66</v>
       </c>
       <c r="D9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E9">
-        <v>12.5</v>
+        <v>34.3</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -2960,10 +2984,10 @@
         <v>67</v>
       </c>
       <c r="D10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10">
-        <v>50.0</v>
+        <v>25.0</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2977,10 +3001,10 @@
         <v>68</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11">
-        <v>34.38</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -2994,10 +3018,10 @@
         <v>69</v>
       </c>
       <c r="D12">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12">
-        <v>19.32</v>
+        <v>16.67</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3014,7 +3038,7 @@
         <v>3</v>
       </c>
       <c r="E13">
-        <v>9.72</v>
+        <v>21.43</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -3028,10 +3052,10 @@
         <v>71</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E14">
-        <v>47.32</v>
+        <v>34.23</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -3048,7 +3072,7 @@
         <v>2</v>
       </c>
       <c r="E15">
-        <v>57.15</v>
+        <v>29.17</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3062,10 +3086,10 @@
         <v>72</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E16">
-        <v>77.08</v>
+        <v>8.34</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3078,12 +3102,8 @@
       <c r="C17" t="s">
         <v>73</v>
       </c>
-      <c r="D17">
-        <v>3</v>
-      </c>
-      <c r="E17">
-        <v>27.66</v>
-      </c>
+      <c r="D17"/>
+      <c r="E17"/>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" t="s">
@@ -3096,10 +3116,10 @@
         <v>74</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E18">
-        <v>17.71</v>
+        <v>15.03</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -3113,10 +3133,10 @@
         <v>75</v>
       </c>
       <c r="D19">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>14.29</v>
+        <v>63.89</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3130,10 +3150,10 @@
         <v>76</v>
       </c>
       <c r="D20">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E20">
-        <v>27.68</v>
+        <v>85.42</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -3150,7 +3170,7 @@
         <v>3</v>
       </c>
       <c r="E21">
-        <v>42.71</v>
+        <v>11.46</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -3542,8 +3562,12 @@
       <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="D11"/>
-      <c r="E11"/>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
@@ -3559,7 +3583,7 @@
         <v>2</v>
       </c>
       <c r="E12">
-        <v>3.13</v>
+        <v>52.09</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -3572,8 +3596,12 @@
       <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="D13"/>
-      <c r="E13"/>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>69.64</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
@@ -3599,10 +3627,10 @@
         <v>19</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15">
-        <v>21.88</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -3619,7 +3647,7 @@
         <v>2</v>
       </c>
       <c r="E16">
-        <v>8.34</v>
+        <v>42.86</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -3633,10 +3661,10 @@
         <v>21</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17">
-        <v>18.18</v>
+        <v>46.43</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -3649,8 +3677,12 @@
       <c r="C18" t="s">
         <v>22</v>
       </c>
-      <c r="D18"/>
-      <c r="E18"/>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>39.29</v>
+      </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
@@ -3663,10 +3695,10 @@
         <v>23</v>
       </c>
       <c r="D19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>26.79</v>
+        <v>57.14</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -3683,7 +3715,7 @@
         <v>2</v>
       </c>
       <c r="E20">
-        <v>53.57</v>
+        <v>172.92</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -3696,12 +3728,8 @@
       <c r="C21" t="s">
         <v>25</v>
       </c>
-      <c r="D21">
-        <v>2</v>
-      </c>
-      <c r="E21">
-        <v>30.36</v>
-      </c>
+      <c r="D21"/>
+      <c r="E21"/>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" t="s">
@@ -3713,8 +3741,12 @@
       <c r="C22" t="s">
         <v>26</v>
       </c>
-      <c r="D22"/>
-      <c r="E22"/>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
@@ -3726,8 +3758,12 @@
       <c r="C23" t="s">
         <v>27</v>
       </c>
-      <c r="D23"/>
-      <c r="E23"/>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>8.33</v>
+      </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" t="s">
@@ -3740,10 +3776,10 @@
         <v>28</v>
       </c>
       <c r="D24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>12.5</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -3756,12 +3792,8 @@
       <c r="C25" t="s">
         <v>29</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>21.43</v>
-      </c>
+      <c r="D25"/>
+      <c r="E25"/>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" t="s">
@@ -3790,7 +3822,7 @@
         <v>2</v>
       </c>
       <c r="E27">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -3807,7 +3839,7 @@
         <v>2</v>
       </c>
       <c r="E28">
-        <v>89.13</v>
+        <v>70.84</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -3820,8 +3852,12 @@
       <c r="C29" t="s">
         <v>33</v>
       </c>
-      <c r="D29"/>
-      <c r="E29"/>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29">
+        <v>37.5</v>
+      </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" t="s">
@@ -3833,12 +3869,8 @@
       <c r="C30" t="s">
         <v>34</v>
       </c>
-      <c r="D30">
-        <v>2</v>
-      </c>
-      <c r="E30">
-        <v>3.13</v>
-      </c>
+      <c r="D30"/>
+      <c r="E30"/>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" t="s">
@@ -4281,8 +4313,12 @@
       <c r="C8" t="s">
         <v>15</v>
       </c>
-      <c r="D8"/>
-      <c r="E8"/>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>0.0</v>
+      </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
@@ -4295,10 +4331,10 @@
         <v>66</v>
       </c>
       <c r="D9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>3.13</v>
+        <v>60.87</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -4325,10 +4361,10 @@
         <v>68</v>
       </c>
       <c r="D11">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E11">
-        <v>15.11</v>
+        <v>27.68</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -4342,10 +4378,10 @@
         <v>69</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12">
-        <v>18.18</v>
+        <v>46.43</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -4358,8 +4394,12 @@
       <c r="C13" t="s">
         <v>70</v>
       </c>
-      <c r="D13"/>
-      <c r="E13"/>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>39.29</v>
+      </c>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
@@ -4372,10 +4412,10 @@
         <v>71</v>
       </c>
       <c r="D14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E14">
-        <v>40.18</v>
+        <v>115.03</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -4388,12 +4428,8 @@
       <c r="C15" t="s">
         <v>25</v>
       </c>
-      <c r="D15">
-        <v>2</v>
-      </c>
-      <c r="E15">
-        <v>30.36</v>
-      </c>
+      <c r="D15"/>
+      <c r="E15"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
@@ -4405,8 +4441,12 @@
       <c r="C16" t="s">
         <v>72</v>
       </c>
-      <c r="D16"/>
-      <c r="E16"/>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>4.17</v>
+      </c>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" t="s">
@@ -4419,10 +4459,10 @@
         <v>73</v>
       </c>
       <c r="D17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>12.5</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -4435,12 +4475,8 @@
       <c r="C18" t="s">
         <v>74</v>
       </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>21.43</v>
-      </c>
+      <c r="D18"/>
+      <c r="E18"/>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
@@ -4456,7 +4492,7 @@
         <v>2</v>
       </c>
       <c r="E19">
-        <v>0.0</v>
+        <v>50.0</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -4473,7 +4509,7 @@
         <v>2</v>
       </c>
       <c r="E20">
-        <v>89.13</v>
+        <v>70.84</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -4490,7 +4526,7 @@
         <v>2</v>
       </c>
       <c r="E21">
-        <v>3.13</v>
+        <v>37.5</v>
       </c>
     </row>
     <row r="22" spans="1:6">

</xml_diff>